<commit_message>
Data en .dat y configuracion Jaula/AGC
- La data ahora se carga desde archivos .dat
- Se agregaron opciones para activar y desactivar la jaula y el AGC en cada maquina
</commit_message>
<xml_diff>
--- a/Datos9barras.xlsx
+++ b/Datos9barras.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Google Drive\Conversión y Transporte de Energía\CT4211 - Potencia III\SepDic2017 - Prof. Bermudez\Programas\Estabilidad-Transitoria-PIII\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Montilva\Google Drive\Conversión y Transporte de Energía\CT4211 - Potencia III\SepDic2017 - Prof. Bermudez\Programas\Estabilidad-Transitoria-PIII\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775" tabRatio="883" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775" tabRatio="883" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="NODOS" sheetId="2" r:id="rId1"/>
@@ -1456,7 +1456,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,6 +1730,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2302,8 +2303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,19 +2420,20 @@
         <v>1</v>
       </c>
       <c r="O2" s="5">
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="P2" s="5">
         <v>1</v>
       </c>
       <c r="Q2" s="27">
-        <v>2.4</v>
+        <f>0.9696</f>
+        <v>0.96960000000000002</v>
       </c>
       <c r="R2" s="28">
         <v>0.1</v>
       </c>
-      <c r="S2" s="28">
-        <v>2</v>
+      <c r="S2" s="5">
+        <v>0.9</v>
       </c>
       <c r="T2" s="5">
         <v>2</v>
@@ -2487,13 +2489,14 @@
         <v>1</v>
       </c>
       <c r="Q3" s="27">
-        <v>2.4</v>
+        <f>1.25</f>
+        <v>1.25</v>
       </c>
       <c r="R3" s="28">
         <v>0.1</v>
       </c>
-      <c r="S3" s="28">
-        <v>2</v>
+      <c r="S3" s="5">
+        <v>0.9</v>
       </c>
       <c r="T3" s="5">
         <v>2</v>
@@ -2549,13 +2552,14 @@
         <v>1</v>
       </c>
       <c r="Q4" s="27">
-        <v>2.4</v>
+        <f>1.875</f>
+        <v>1.875</v>
       </c>
       <c r="R4" s="28">
         <v>0.1</v>
       </c>
-      <c r="S4" s="28">
-        <v>2</v>
+      <c r="S4" s="5">
+        <v>0.9</v>
       </c>
       <c r="T4" s="5">
         <v>2</v>
@@ -2574,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2703,7 +2707,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="30">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>